<commit_message>
finished grading per subject
</commit_message>
<xml_diff>
--- a/documents/excel/Expected_screened_client_table_data_format (1).xlsx
+++ b/documents/excel/Expected_screened_client_table_data_format (1).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
   <si>
     <t>SN</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>test@test.com</t>
+  </si>
+  <si>
+    <t>odenadoma@gmail.com</t>
+  </si>
+  <si>
+    <t>greyspades99@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -503,7 +509,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,7 +582,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>28</v>
@@ -608,7 +614,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>29</v>
@@ -640,7 +646,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>30</v>
@@ -873,8 +879,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>